<commit_message>
-Adding excel comparisons and general changes
</commit_message>
<xml_diff>
--- a/content/blog/2020-07-31-spreadsheet-workflows-using-r/data/spending.xlsx
+++ b/content/blog/2020-07-31-spreadsheet-workflows-using-r/data/spending.xlsx
@@ -5,21 +5,28 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/spareaccount/Desktop/article pre git/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/devin/Desktop/github/education.rstudio.com/content/blog/2020-07-31-spreadsheet-workflows-using-r/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{54B93589-3A8C-254D-9A62-1F437187713D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{F8ED5F68-3FC0-D543-9C43-F2A4924BFC5D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="40" yWindow="460" windowWidth="28760" windowHeight="16220" xr2:uid="{EFFA5C92-796B-BD48-B3E6-2E2040885210}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -456,8 +463,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{62C1EBD2-AF89-1649-9CEE-3A446E1DA07E}">
   <dimension ref="A1:E49"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1304,18 +1311,4 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{56424881-4413-C746-AD2A-839C6D4FA5E3}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>